<commit_message>
Fix table sorting, fix book add info, prevent duplicates
</commit_message>
<xml_diff>
--- a/static/data/bookdata.xlsx
+++ b/static/data/bookdata.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jarem\Desktop\data_science\python-working-directory\_MyApps\BookClub2.0\static\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C72287F0-469F-4322-B1AF-CBB760555B5E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4A423225-FB93-4723-88F3-D91587D24AAF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -18106,8 +18106,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G2772"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2753" workbookViewId="0">
-      <selection activeCell="A2773" sqref="A2773:XFD2774"/>
+    <sheetView tabSelected="1" topLeftCell="A2761" workbookViewId="0">
+      <selection activeCell="J2775" sqref="J2775"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>